<commit_message>
Biomerieux 14/03/2017 sheet order fixed
</commit_message>
<xml_diff>
--- a/data/Biomerieux.xlsx
+++ b/data/Biomerieux.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120" firstSheet="9" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="17 02 2017" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <sheet name="02 03 2017" sheetId="10" r:id="rId10"/>
     <sheet name="03 03 2017" sheetId="11" r:id="rId11"/>
     <sheet name="06 03 2017" sheetId="12" r:id="rId12"/>
-    <sheet name="14 03 2017" sheetId="13" r:id="rId13"/>
-    <sheet name="07 03 2017" sheetId="14" r:id="rId14"/>
-    <sheet name="08 03 2017" sheetId="15" r:id="rId15"/>
-    <sheet name="09 03 2017" sheetId="16" r:id="rId16"/>
-    <sheet name="10 03 2017" sheetId="17" r:id="rId17"/>
-    <sheet name="13 03 2017" sheetId="18" r:id="rId18"/>
+    <sheet name="07 03 2017" sheetId="14" r:id="rId13"/>
+    <sheet name="08 03 2017" sheetId="15" r:id="rId14"/>
+    <sheet name="09 03 2017" sheetId="16" r:id="rId15"/>
+    <sheet name="10 03 2017" sheetId="17" r:id="rId16"/>
+    <sheet name="13 03 2017" sheetId="18" r:id="rId17"/>
+    <sheet name="14 03 2017" sheetId="13" r:id="rId18"/>
     <sheet name="15 03 2017" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -789,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -862,7 +862,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.15075000000000002</v>
+        <v>5.5550000000000009E-2</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -971,11 +971,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.45</v>
+        <v>-0.11</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>7.6500000000000012E-2</v>
+        <v>-1.8700000000000001E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1778,7 +1778,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.42210000000000003</v>
+        <v>0.36770000000000003</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1887,11 +1887,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.98</v>
+        <v>0.66</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>0.1666</v>
+        <v>0.11220000000000001</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2642,7 +2642,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.27950000000000003</v>
+        <v>0.15539999999999998</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2751,11 +2751,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.1</v>
+        <v>-0.63</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>1.7000000000000001E-2</v>
+        <v>-0.10710000000000001</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3508,7 +3508,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>4.4399999999999995E-2</v>
+        <v>0.2722</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -3617,11 +3617,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>-0.48</v>
+        <v>0.86</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>-8.1600000000000006E-2</v>
+        <v>0.1462</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4316,7 +4316,7 @@
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="101" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="17" width="7.42578125" customWidth="1"/>
@@ -4377,12 +4377,12 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.13739999999999999</v>
+        <v>-8.9000000000000024E-2</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -4413,16 +4413,16 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(D11:D15)</f>
-        <v>1.9999999999999976E-2</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="D3" s="2">
         <f>B3*C3</f>
-        <v>4.4999999999999945E-3</v>
+        <v>-3.1500000000000007E-2</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -4491,11 +4491,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.12</v>
+        <v>-1</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>2.0400000000000001E-2</v>
+        <v>-0.17</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4678,14 +4678,14 @@
         <v>0.2</v>
       </c>
       <c r="C11" s="5">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="D11" s="2">
         <f>B11*C11</f>
-        <v>4.0000000000000008E-2</v>
+        <v>-4.0000000000000008E-2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -4717,14 +4717,14 @@
         <v>0.2</v>
       </c>
       <c r="C12" s="5">
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2">
         <f>B12*C12</f>
-        <v>-8.0000000000000016E-2</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>68</v>
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -4756,14 +4756,14 @@
         <v>0.2</v>
       </c>
       <c r="C13" s="5">
-        <v>-0.4</v>
+        <v>-0.2</v>
       </c>
       <c r="D13" s="2">
         <f>B13*C13</f>
-        <v>-8.0000000000000016E-2</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>69</v>
+        <v>-4.0000000000000008E-2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -4795,14 +4795,14 @@
         <v>0.2</v>
       </c>
       <c r="C14" s="5">
-        <v>0.6</v>
+        <v>-0.3</v>
       </c>
       <c r="D14" s="2">
         <f>B14*C14</f>
-        <v>0.12</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>70</v>
+        <v>-0.06</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -4834,14 +4834,14 @@
         <v>0.2</v>
       </c>
       <c r="C15" s="5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
         <f>B15*C15</f>
-        <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>71</v>
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>30</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -5001,9 +5001,7 @@
         <f>B20*C20</f>
         <v>0.2</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -5026,7 +5024,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -5040,9 +5038,7 @@
         <f>B21*C21</f>
         <v>-0.1</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -5079,9 +5075,7 @@
         <f>B22*C22</f>
         <v>0.1</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -5118,9 +5112,7 @@
         <f>B23*C23</f>
         <v>0.1</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -5157,9 +5149,7 @@
         <f>B24*C24</f>
         <v>0.2</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -5261,12 +5251,12 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.2306</v>
+        <v>0.2359</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -5297,16 +5287,16 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(D11:D15)</f>
-        <v>-0.14000000000000001</v>
+        <v>-0.12400000000000001</v>
       </c>
       <c r="D3" s="2">
         <f>B3*C3</f>
-        <v>-3.1500000000000007E-2</v>
+        <v>-2.7900000000000005E-2</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -5375,11 +5365,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>0.14960000000000001</v>
+        <v>0.15130000000000002</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -5562,11 +5552,11 @@
         <v>0.2</v>
       </c>
       <c r="C11" s="5">
-        <v>-0.2</v>
+        <v>-0.02</v>
       </c>
       <c r="D11" s="2">
         <f>B11*C11</f>
-        <v>-4.0000000000000008E-2</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>34</v>
@@ -5601,14 +5591,14 @@
         <v>0.2</v>
       </c>
       <c r="C12" s="5">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D12" s="2">
         <f>B12*C12</f>
-        <v>0</v>
+        <v>-2.0000000000000004E-2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -5647,7 +5637,7 @@
         <v>-4.0000000000000008E-2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -5724,8 +5714,8 @@
         <f>B15*C15</f>
         <v>0</v>
       </c>
-      <c r="E15" s="2">
-        <v>30</v>
+      <c r="E15" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -5885,7 +5875,9 @@
         <f>B20*C20</f>
         <v>0.2</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -5908,7 +5900,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -5922,7 +5914,9 @@
         <f>B21*C21</f>
         <v>-0.1</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -5959,7 +5953,9 @@
         <f>B22*C22</f>
         <v>0.1</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -5996,7 +5992,9 @@
         <f>B23*C23</f>
         <v>0.1</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -6033,7 +6031,9 @@
         <f>B24*C24</f>
         <v>0.2</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -6074,7 +6074,7 @@
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="48.85546875" customWidth="1"/>
+    <col min="5" max="5" width="102.85546875" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="17" width="7.42578125" customWidth="1"/>
@@ -6140,7 +6140,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>8.9700000000000002E-2</v>
+        <v>0.19160000000000002</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -6171,11 +6171,11 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(D11:D15)</f>
-        <v>-0.12400000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D3" s="2">
         <f>B3*C3</f>
-        <v>-2.7900000000000005E-2</v>
+        <v>3.1500000000000007E-2</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -6249,11 +6249,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.03</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>5.1000000000000004E-3</v>
+        <v>4.760000000000001E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -6436,14 +6436,14 @@
         <v>0.2</v>
       </c>
       <c r="C11" s="5">
-        <v>-0.02</v>
+        <v>0.3</v>
       </c>
       <c r="D11" s="2">
         <f>B11*C11</f>
-        <v>-4.0000000000000001E-3</v>
+        <v>0.06</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -6475,14 +6475,14 @@
         <v>0.2</v>
       </c>
       <c r="C12" s="5">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2">
         <f>B12*C12</f>
-        <v>-2.0000000000000004E-2</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -6514,14 +6514,14 @@
         <v>0.2</v>
       </c>
       <c r="C13" s="5">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="D13" s="2">
         <f>B13*C13</f>
-        <v>-4.0000000000000008E-2</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>34</v>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -6553,14 +6553,14 @@
         <v>0.2</v>
       </c>
       <c r="C14" s="5">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2">
         <f>B14*C14</f>
-        <v>-0.06</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -6592,14 +6592,14 @@
         <v>0.2</v>
       </c>
       <c r="C15" s="5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D15" s="2">
         <f>B15*C15</f>
-        <v>0</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -6958,7 +6958,7 @@
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="102.85546875" customWidth="1"/>
+    <col min="5" max="5" width="89.140625" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="17" width="7.42578125" customWidth="1"/>
@@ -7024,7 +7024,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.21880000000000002</v>
+        <v>9.290000000000001E-2</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -7055,11 +7055,11 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(D11:D15)</f>
-        <v>0.14000000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="D3" s="2">
         <f>B3*C3</f>
-        <v>3.1500000000000007E-2</v>
+        <v>0.12150000000000001</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -7133,11 +7133,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.44</v>
+        <v>-0.83</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>7.4800000000000005E-2</v>
+        <v>-0.1411</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -7320,14 +7320,14 @@
         <v>0.2</v>
       </c>
       <c r="C11" s="5">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="2">
         <f>B11*C11</f>
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -7359,14 +7359,14 @@
         <v>0.2</v>
       </c>
       <c r="C12" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D12" s="2">
         <f>B12*C12</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>74</v>
+        <v>8.0000000000000016E-2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -7398,14 +7398,14 @@
         <v>0.2</v>
       </c>
       <c r="C13" s="5">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="D13" s="2">
         <f>B13*C13</f>
-        <v>4.0000000000000008E-2</v>
+        <v>0.13999999999999999</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -7437,14 +7437,14 @@
         <v>0.2</v>
       </c>
       <c r="C14" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D14" s="2">
         <f>B14*C14</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>76</v>
+        <v>8.0000000000000016E-2</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -7476,14 +7476,14 @@
         <v>0.2</v>
       </c>
       <c r="C15" s="5">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="D15" s="2">
         <f>B15*C15</f>
-        <v>4.0000000000000008E-2</v>
+        <v>0.13999999999999999</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -7842,7 +7842,7 @@
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="89.140625" customWidth="1"/>
+    <col min="5" max="5" width="102.5703125" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="17" width="7.42578125" customWidth="1"/>
@@ -7908,7 +7908,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.27140000000000003</v>
+        <v>0.25880000000000003</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -7939,11 +7939,11 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(D11:D15)</f>
-        <v>0.54</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D3" s="2">
         <f>B3*C3</f>
-        <v>0.12150000000000001</v>
+        <v>6.3000000000000014E-2</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -8017,11 +8017,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.22</v>
+        <v>0.49</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>3.7400000000000003E-2</v>
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -8204,14 +8204,14 @@
         <v>0.2</v>
       </c>
       <c r="C11" s="5">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D11" s="2">
         <f>B11*C11</f>
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -8243,14 +8243,14 @@
         <v>0.2</v>
       </c>
       <c r="C12" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D12" s="2">
         <f>B12*C12</f>
-        <v>8.0000000000000016E-2</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -8282,14 +8282,14 @@
         <v>0.2</v>
       </c>
       <c r="C13" s="5">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="D13" s="2">
         <f>B13*C13</f>
-        <v>0.13999999999999999</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -8321,14 +8321,14 @@
         <v>0.2</v>
       </c>
       <c r="C14" s="5">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D14" s="2">
         <f>B14*C14</f>
-        <v>8.0000000000000016E-2</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>80</v>
+        <v>0.06</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -8360,14 +8360,14 @@
         <v>0.2</v>
       </c>
       <c r="C15" s="5">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="D15" s="2">
         <f>B15*C15</f>
-        <v>0.13999999999999999</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>81</v>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -8719,14 +8719,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="102.5703125" customWidth="1"/>
+    <col min="5" max="5" width="101" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="17" width="7.42578125" customWidth="1"/>
@@ -8792,7 +8792,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.24350000000000002</v>
+        <v>0.22070000000000001</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -8823,11 +8823,11 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(D11:D15)</f>
-        <v>0.28000000000000003</v>
+        <v>1.9999999999999976E-2</v>
       </c>
       <c r="D3" s="2">
         <f>B3*C3</f>
-        <v>6.3000000000000014E-2</v>
+        <v>4.4999999999999945E-3</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -8901,11 +8901,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.4</v>
+        <v>0.61</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>6.8000000000000005E-2</v>
+        <v>0.1037</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -9088,11 +9088,11 @@
         <v>0.2</v>
       </c>
       <c r="C11" s="5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D11" s="2">
         <f>B11*C11</f>
-        <v>0.06</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>67</v>
@@ -9127,14 +9127,14 @@
         <v>0.2</v>
       </c>
       <c r="C12" s="5">
-        <v>0.2</v>
+        <v>-0.4</v>
       </c>
       <c r="D12" s="2">
         <f>B12*C12</f>
-        <v>4.0000000000000008E-2</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>82</v>
+        <v>-8.0000000000000016E-2</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -9166,14 +9166,14 @@
         <v>0.2</v>
       </c>
       <c r="C13" s="5">
-        <v>0.4</v>
+        <v>-0.4</v>
       </c>
       <c r="D13" s="2">
         <f>B13*C13</f>
-        <v>8.0000000000000016E-2</v>
+        <v>-8.0000000000000016E-2</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -9205,13 +9205,13 @@
         <v>0.2</v>
       </c>
       <c r="C14" s="5">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="D14" s="2">
         <f>B14*C14</f>
-        <v>0.06</v>
-      </c>
-      <c r="E14" s="9" t="s">
+        <v>0.12</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>70</v>
       </c>
       <c r="F14" s="2"/>
@@ -9244,11 +9244,11 @@
         <v>0.2</v>
       </c>
       <c r="C15" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D15" s="2">
         <f>B15*C15</f>
-        <v>4.0000000000000008E-2</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>71</v>
@@ -9676,7 +9676,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.32830000000000004</v>
+        <v>0.19060000000000002</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -9785,11 +9785,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.74</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>0.1258</v>
+        <v>-1.1900000000000003E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -10560,7 +10560,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.33875000000000005</v>
+        <v>0.33705000000000007</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -10669,11 +10669,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>0.1275</v>
+        <v>0.1258</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -11444,7 +11444,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.32879999999999998</v>
+        <v>0.4546</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -11553,11 +11553,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.19</v>
+        <v>0.93</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>3.2300000000000002E-2</v>
+        <v>0.15810000000000002</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -12328,7 +12328,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.30149999999999999</v>
+        <v>0.35420000000000001</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -12437,11 +12437,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.4</v>
+        <v>0.71</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>6.8000000000000005E-2</v>
+        <v>0.1207</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -13209,7 +13209,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.35660000000000003</v>
+        <v>0.38040000000000002</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -13318,11 +13318,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.57999999999999996</v>
+        <v>0.72</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>9.8600000000000007E-2</v>
+        <v>0.12240000000000001</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -14081,7 +14081,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.3155</v>
+        <v>0.154</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -14190,11 +14190,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.3</v>
+        <v>-0.65</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>5.1000000000000004E-2</v>
+        <v>-0.11050000000000001</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -14949,7 +14949,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.32980000000000004</v>
+        <v>0.25840000000000007</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -15058,11 +15058,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.54</v>
+        <v>0.12</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>9.1800000000000007E-2</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -15817,7 +15817,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.33879999999999999</v>
+        <v>0.1076</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -15926,11 +15926,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.54</v>
+        <v>-0.82</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>9.1800000000000007E-2</v>
+        <v>-0.1394</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -16685,7 +16685,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2">
         <f ca="1">SUM(D2:D5)</f>
-        <v>0.41589999999999999</v>
+        <v>0.39889999999999998</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -16794,11 +16794,11 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(-100,100) / 100</f>
-        <v>0.27</v>
+        <v>0.17</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5*C5</f>
-        <v>4.5900000000000003E-2</v>
+        <v>2.8900000000000006E-2</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>

</xml_diff>